<commit_message>
Frontend changes for API response update
</commit_message>
<xml_diff>
--- a/Reports/Gantt Chart.xlsx
+++ b/Reports/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSIS\static-code-analysis\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEC6E1C-4E7F-475B-B061-41A04BFACF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC4025F-C7B6-4277-A238-CD278F8AE196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,12 +177,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -256,8 +250,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,10 +261,6 @@
     <xf numFmtId="17" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +544,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +561,7 @@
     <col min="11" max="11" width="7.54296875" customWidth="1"/>
     <col min="14" max="14" width="8.08984375" customWidth="1"/>
     <col min="16" max="16" width="3.26953125" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
@@ -642,25 +632,25 @@
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="O3" s="1"/>
@@ -982,7 +972,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="2"/>
@@ -1005,7 +995,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="16"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1026,7 +1016,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="2"/>
@@ -1036,7 +1026,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="4"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1049,7 +1039,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1070,7 +1060,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="2"/>
@@ -1082,8 +1072,8 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
       <c r="N22" s="2"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1093,7 +1083,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
-      <c r="B23" s="16"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1114,7 +1104,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="2"/>
@@ -1127,8 +1117,8 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1137,7 +1127,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="16"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1158,7 +1148,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="3"/>
@@ -1167,12 +1157,12 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>

</xml_diff>